<commit_message>
Added short pulse filter to filter out high speed anomalies
</commit_message>
<xml_diff>
--- a/speedo_cal.xlsx
+++ b/speedo_cal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boult\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\Chevy_speedo_interceptor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C19865-664C-4896-89C6-E3453A55E25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85EFD40-C724-438E-8C75-8A3981BF207B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20271" yWindow="523" windowWidth="3180" windowHeight="10946" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1249,7 +1249,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1422,7 +1422,37 @@
         <v>6428</v>
       </c>
     </row>
-    <row r="33" spans="13:13" x14ac:dyDescent="0.4">
+    <row r="30" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D30">
+        <v>150</v>
+      </c>
+      <c r="E30">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D31">
+        <v>160</v>
+      </c>
+      <c r="E31">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D32">
+        <v>170</v>
+      </c>
+      <c r="E32">
+        <v>5294</v>
+      </c>
+    </row>
+    <row r="33" spans="4:13" x14ac:dyDescent="0.4">
+      <c r="D33">
+        <v>180</v>
+      </c>
+      <c r="E33">
+        <v>5000</v>
+      </c>
       <c r="M33">
         <v>0</v>
       </c>

</xml_diff>